<commit_message>
update and do some modify
11111
</commit_message>
<xml_diff>
--- a/速贷后台测试场景_V0.1.xlsx
+++ b/速贷后台测试场景_V0.1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larrychiou/Documents/速贷/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" tabRatio="500"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <sheet name="审核记录" sheetId="5" r:id="rId5"/>
     <sheet name="贷后信息查询" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1666,6 +1661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1676,13 +1672,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1737,7 +1732,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1772,7 +1767,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1949,7 +1944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1957,29 +1952,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E16"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
+      <c r="B2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5">
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="D6" t="s">
         <v>1</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5">
       <c r="D7" t="s">
         <v>7</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:5">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:5">
       <c r="D9" t="s">
         <v>3</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:5">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -2022,12 +2022,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:5">
       <c r="D12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:5">
       <c r="B16" t="s">
         <v>107</v>
       </c>
@@ -2038,6 +2038,11 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2049,13 +2054,13 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2063,7 +2068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2071,17 +2076,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="B3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="C5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2098,7 +2103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2109,7 +2114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
         <v>22</v>
@@ -2120,7 +2125,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
@@ -2131,7 +2136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2144,7 +2149,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
         <v>22</v>
@@ -2157,7 +2162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
@@ -2170,7 +2175,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2185,7 +2190,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2197,6 +2202,11 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2208,14 +2218,14 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -2223,7 +2233,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="B3">
         <v>1</v>
       </c>
@@ -2234,7 +2244,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="B4">
         <v>2</v>
       </c>
@@ -2245,44 +2255,44 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="B5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C6" s="17" t="s">
+    <row r="6" spans="1:4">
+      <c r="C6" s="18" t="s">
         <v>82</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C7" s="17"/>
+    <row r="7" spans="1:4">
+      <c r="C7" s="18"/>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C8" s="17"/>
+    <row r="8" spans="1:4">
+      <c r="C8" s="18"/>
       <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C9" s="17"/>
+    <row r="9" spans="1:4">
+      <c r="C9" s="18"/>
       <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C10" s="17"/>
+    <row r="10" spans="1:4">
+      <c r="C10" s="18"/>
       <c r="D10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="B11">
         <v>4</v>
       </c>
@@ -2290,66 +2300,66 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C12" s="17" t="s">
+    <row r="12" spans="1:4">
+      <c r="C12" s="18" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C13" s="17"/>
+    <row r="13" spans="1:4">
+      <c r="C13" s="18"/>
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C14" s="17"/>
+    <row r="14" spans="1:4">
+      <c r="C14" s="18"/>
       <c r="D14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C15" s="17"/>
+    <row r="15" spans="1:4">
+      <c r="C15" s="18"/>
       <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="C16" s="17"/>
+    <row r="16" spans="1:4">
+      <c r="C16" s="18"/>
       <c r="D16" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C17" s="17"/>
+    <row r="17" spans="2:4">
+      <c r="C17" s="18"/>
       <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C18" s="17"/>
+    <row r="18" spans="2:4">
+      <c r="C18" s="18"/>
       <c r="D18" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C19" s="17"/>
+    <row r="19" spans="2:4">
+      <c r="C19" s="18"/>
       <c r="D19" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C20" s="17"/>
+    <row r="20" spans="2:4">
+      <c r="C20" s="18"/>
       <c r="D20" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:4">
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:4">
       <c r="B22">
         <v>5</v>
       </c>
@@ -2360,7 +2370,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:4">
       <c r="B24">
         <v>6</v>
       </c>
@@ -2371,27 +2381,27 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:4">
       <c r="B26">
         <v>7</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="18" t="s">
         <v>85</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C27" s="17"/>
+    <row r="27" spans="2:4">
+      <c r="C27" s="18"/>
       <c r="D27" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:4">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:4">
       <c r="B29">
         <v>8</v>
       </c>
@@ -2402,68 +2412,68 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:4">
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:4">
       <c r="B31">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C32" s="17" t="s">
+    <row r="32" spans="2:4">
+      <c r="C32" s="18" t="s">
         <v>87</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C33" s="17"/>
+    <row r="33" spans="2:4">
+      <c r="C33" s="18"/>
       <c r="D33" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C34" s="17"/>
+    <row r="34" spans="2:4">
+      <c r="C34" s="18"/>
       <c r="D34" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C35" s="17"/>
+    <row r="35" spans="2:4">
+      <c r="C35" s="18"/>
       <c r="D35" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C36" s="17"/>
+    <row r="36" spans="2:4">
+      <c r="C36" s="18"/>
       <c r="D36" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C37" s="17"/>
+    <row r="37" spans="2:4">
+      <c r="C37" s="18"/>
       <c r="D37" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C38" s="17"/>
+    <row r="38" spans="2:4">
+      <c r="C38" s="18"/>
       <c r="D38" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C39" s="17"/>
+    <row r="39" spans="2:4">
+      <c r="C39" s="18"/>
       <c r="D39" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:4">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:4">
       <c r="B41">
         <v>10</v>
       </c>
@@ -2474,67 +2484,72 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:4">
       <c r="B42">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C43" s="17" t="s">
+    <row r="43" spans="2:4">
+      <c r="C43" s="18" t="s">
         <v>66</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C44" s="17"/>
+    <row r="44" spans="2:4">
+      <c r="C44" s="18"/>
       <c r="D44" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C45" s="17"/>
+    <row r="45" spans="2:4">
+      <c r="C45" s="18"/>
       <c r="D45" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C46" s="17"/>
+    <row r="46" spans="2:4">
+      <c r="C46" s="18"/>
       <c r="D46" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:4">
       <c r="B47">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C48" s="17" t="s">
+    <row r="48" spans="2:4">
+      <c r="C48" s="18" t="s">
         <v>67</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C49" s="17"/>
+    <row r="49" spans="3:4">
+      <c r="C49" s="18"/>
       <c r="D49" s="2" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C48:C49"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="C12:C20"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C32:C39"/>
     <mergeCell ref="C43:C46"/>
-    <mergeCell ref="C48:C49"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2546,14 +2561,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="40.1640625" customWidth="1"/>
     <col min="4" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2561,7 +2576,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2569,7 +2584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="C4" s="8"/>
       <c r="D4" s="4"/>
       <c r="E4" s="9" t="s">
@@ -2580,58 +2595,58 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C5" s="19" t="s">
+    <row r="5" spans="1:7">
+      <c r="C5" s="20" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C6" s="19"/>
+    <row r="6" spans="1:7">
+      <c r="C6" s="20"/>
       <c r="D6" s="5"/>
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C7" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" s="20"/>
       <c r="D7" s="5"/>
       <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C8" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8" s="20"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C9" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9" s="21"/>
       <c r="D9" s="6"/>
       <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F9" s="21"/>
+      <c r="G9" s="19"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="9" t="s">
@@ -2640,116 +2655,116 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C13" s="20" t="s">
+    <row r="13" spans="1:7">
+      <c r="C13" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="21" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+    <row r="14" spans="1:7">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+    </row>
+    <row r="24" spans="2:7">
       <c r="E24" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7">
       <c r="E25" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7">
       <c r="E26" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:7">
       <c r="B29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:7">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="9"/>
@@ -2758,92 +2773,92 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C31" s="18" t="s">
+    <row r="31" spans="2:7">
+      <c r="C31" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="19" t="s">
         <v>52</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
+    <row r="32" spans="2:7">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="3:9">
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="3:9">
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
       <c r="F34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="3:9">
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
+      <c r="G35" s="19"/>
+    </row>
+    <row r="36" spans="3:9">
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="18"/>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
+      <c r="G36" s="19"/>
+    </row>
+    <row r="37" spans="3:9">
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="3:9">
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G38" s="18"/>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="G38" s="19"/>
+    </row>
+    <row r="44" spans="3:9">
       <c r="C44" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="3:9">
       <c r="C45" s="2" t="s">
         <v>66</v>
       </c>
@@ -2866,10 +2881,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="3:9">
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="3:9">
       <c r="C47" s="2" t="s">
         <v>67</v>
       </c>
@@ -2902,6 +2917,11 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2913,9 +2933,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="45">
       <c r="A2" s="10" t="s">
         <v>78</v>
       </c>
@@ -2923,7 +2943,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="120">
       <c r="A3" s="10" t="s">
         <v>113</v>
       </c>
@@ -2931,7 +2951,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16">
       <c r="B4" t="s">
         <v>110</v>
       </c>
@@ -2953,11 +2973,11 @@
       <c r="H4" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2968,7 +2988,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2977,7 +2997,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2986,7 +3006,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2995,7 +3015,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -3004,7 +3024,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3013,7 +3033,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -3022,7 +3042,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -3031,7 +3051,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -3040,7 +3060,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -3049,7 +3069,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -3058,7 +3078,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -3067,7 +3087,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:9">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3076,7 +3096,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:9">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -3085,7 +3105,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:9">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -3094,7 +3114,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:9">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -3103,7 +3123,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:9">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -3112,7 +3132,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="22"/>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:9">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -3121,7 +3141,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="22"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="3:9">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -3136,6 +3156,11 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3147,14 +3172,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="31.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="49.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -3162,7 +3187,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="105">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -3170,7 +3195,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="C3" t="s">
         <v>116</v>
       </c>
@@ -3178,5 +3203,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>